<commit_message>
Update AchievementsList and Levels17MoveList. ChatEngine: Update dialogue. AchievementSuperEfficient: Update requirement to 22.
</commit_message>
<xml_diff>
--- a/JSON/AchievementsList.xlsx
+++ b/JSON/AchievementsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9143296-D45F-5F4D-A8DD-9DF0864B4DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E149252-54BF-C049-9747-546EE31EE036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46760" yWindow="700" windowWidth="27640" windowHeight="16940" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +780,7 @@
         <v>474</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Achievement requirements for: BeastMaster, BoulderBreaker, DragonSlayer, Exterminator, MyPreciouses, RockNRoller - made it so you need a second playthrough to acquire these.
</commit_message>
<xml_diff>
--- a/JSON/AchievementsList.xlsx
+++ b/JSON/AchievementsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E149252-54BF-C049-9747-546EE31EE036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F39DB-1DBA-864B-B371-93F2F0353A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46760" yWindow="700" windowWidth="27640" windowHeight="16940" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>40?</t>
   </si>
   <si>
-    <t>350?</t>
-  </si>
-  <si>
     <t>Hoarder</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Achievement</t>
+  </si>
+  <si>
+    <t>400?</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,21 +545,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>307</v>
@@ -592,51 +592,51 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>499</v>
+        <v>567</v>
       </c>
       <c r="D5">
-        <v>2800</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>215</v>
+        <v>350</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8">
-        <v>425</v>
+        <v>790</v>
       </c>
       <c r="D8">
-        <v>300</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -647,29 +647,29 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D10">
-        <v>85</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11">
-        <v>400</v>
+        <v>675</v>
       </c>
       <c r="D11">
-        <v>230</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>115</v>
@@ -691,13 +691,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>500</v>
+        <v>790</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Update AchievementsList and Levels17MoveList through 301. AchievementSuperEfficient: update requirement to 30. Update build to 1.19 (20)
</commit_message>
<xml_diff>
--- a/JSON/AchievementsList.xlsx
+++ b/JSON/AchievementsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F39DB-1DBA-864B-B371-93F2F0353A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98895A-322E-1D48-B201-DF3210E41836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +780,7 @@
         <v>474</v>
       </c>
       <c r="D21">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Achievements for BigSpender, EndlessWallet, FatCat: requirements are now $5, $10, $20, respectively.
</commit_message>
<xml_diff>
--- a/JSON/AchievementsList.xlsx
+++ b/JSON/AchievementsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E98895A-322E-1D48-B201-DF3210E41836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B891D882-89E1-734E-8857-1270E3B1A66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Complete Level17MoveList solutions. Update AchievementSuperEfficient to requirement of 35.
</commit_message>
<xml_diff>
--- a/JSON/AchievementsList.xlsx
+++ b/JSON/AchievementsList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B891D882-89E1-734E-8857-1270E3B1A66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4101B04E-5533-4046-A1F6-D269371198DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{CA252AC9-37E4-CD48-B2A1-E26C95CE2AB1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$A$1:$D$30</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,10 +777,11 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>474</v>
+        <f>474+126</f>
+        <v>600</v>
       </c>
       <c r="D21">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>